<commit_message>
constant velocity, obstacles, driver emerg signal
</commit_message>
<xml_diff>
--- a/Dokumentation/Aufwand_dreiPunkt_Methode.xlsx
+++ b/Dokumentation/Aufwand_dreiPunkt_Methode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETAS\workspace\Projekt_Grafische_Programmierung\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA2174C-9B17-4A0B-8461-E9C633F8AD40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE21EF4B-7F43-4CDD-ACE2-5DED09D891D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2403F6F-5791-4371-9394-4C499AB23289}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2403F6F-5791-4371-9394-4C499AB23289}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,6 +561,9 @@
         <f>(E2-C2)^2/36</f>
         <v>100</v>
       </c>
+      <c r="H2">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -586,6 +589,9 @@
         <f t="shared" ref="G3:G12" si="1">(E3-C3)^2/36</f>
         <v>506.25</v>
       </c>
+      <c r="H3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -611,6 +617,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -845,7 +854,7 @@
       </c>
       <c r="H16">
         <f>SUM(H2:H13)</f>
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added all max_count points
</commit_message>
<xml_diff>
--- a/Dokumentation/Aufwand_dreiPunkt_Methode.xlsx
+++ b/Dokumentation/Aufwand_dreiPunkt_Methode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETAS\workspace\Projekt_Grafische_Programmierung\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399FE4E9-A550-4EF6-B739-AF17DC70BB91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9BA21D-3367-4C47-A2F2-5237D1A3C1B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2403F6F-5791-4371-9394-4C499AB23289}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Aufgaben (abgeschätzt)</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Bemerkung</t>
-  </si>
-  <si>
-    <t>Bereits mit Ausweichen umgesetzt</t>
   </si>
 </sst>
 </file>
@@ -502,7 +499,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +707,9 @@
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
+      <c r="H7">
+        <v>120</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -735,12 +735,6 @@
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -765,6 +759,9 @@
       <c r="G9">
         <f t="shared" si="1"/>
         <v>225</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -875,7 +872,7 @@
       </c>
       <c r="H16">
         <f>SUM(H2:H13)</f>
-        <v>560</v>
+        <v>710</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.25">

</xml_diff>